<commit_message>
Added firmware drivers - untested
</commit_message>
<xml_diff>
--- a/Design Files/Output Files/Strelka_Flight_Computer.xlsx
+++ b/Design Files/Output Files/Strelka_Flight_Computer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\OneDrive\Documents\1. Uni Work\HPR\Strelka-Flight-Computer\Design Files\Output Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\Documents\FYP\Strelka-Flight-Computer\Design Files\Output Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA77B69A-46CF-4538-8277-DE0389CEB502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35AF963-808A-47DC-916C-3CB69C73014B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strelka_Flight_Computer" sheetId="1" r:id="rId1"/>
@@ -1970,21 +1970,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="B59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>44877.430555555555</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>2.3124799999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>9.6402999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>8</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>9</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>18</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>19</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>1.11005</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>21</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>1.8774</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>22</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>0.61536999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>24</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>0.41720000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>26</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>2.0405549999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>27</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>0.95061999999999991</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>28</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>29</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0.89399999999999991</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>30</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0.59376499999999988</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>31</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1.8952800000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>32</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0.7420199999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>33</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>0.63325000000000009</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>34</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1.3409999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>35</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.9536</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>36</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0.88655000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>37</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>0.84930000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>39</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>2.1765920000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>40</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>1.5204258000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>41</v>
       </c>
@@ -3244,26 +3244,26 @@
         <v>34.07</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
         <v>42</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="4" t="s">
         <v>341</v>
       </c>
       <c r="J38">
@@ -3278,7 +3278,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>43</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>1.91316</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>44</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>1.9980899999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>45</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>4.3105700000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>46</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>47</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>49</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>2.9442399999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>50</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>0.62699199999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>51</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>0.55726000000000009</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>52</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>0.93274000000000012</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>53</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>54</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>55</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>0.16390000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>56</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0.19369999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>57</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>0.1341</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>58</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>59</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>60</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>61</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>62</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>8.9399999999999993E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>64</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>65</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>2.3685039999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>66</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>0.16390000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>67</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>0.38739999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>70</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>0.20860000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>71</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>0.1341</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>72</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>73</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>0.1341</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>74</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>1.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>75</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>1.60026</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>76</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>1.6464500000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>77</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>78</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>79</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>80</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>41.098967999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>81</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>82</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>1.6735679999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
         <v>83</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>0.64964</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>84</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>47.143599999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>85</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>20.93</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
         <v>86</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>4.5230440000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>87</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>88</v>
       </c>
@@ -4864,17 +4864,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K88" s="6" t="s">
         <v>343</v>
       </c>
@@ -4884,13 +4884,13 @@
         <v>216.35894380000002</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K91" t="s">
         <v>344</v>
       </c>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K92" t="s">
         <v>347</v>
       </c>

</xml_diff>